<commit_message>
generate age-based lookup tables for final TODE sample.
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lswe_sum-raw-ss-lookup-tabbed.xlsx
+++ b/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lswe_sum-raw-ss-lookup-tabbed.xlsx
@@ -382,7 +382,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">
@@ -390,7 +390,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4">
@@ -398,7 +398,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
@@ -406,7 +406,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
@@ -414,7 +414,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7">
@@ -422,7 +422,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8">
@@ -430,7 +430,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9">
@@ -438,7 +438,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10">
@@ -446,7 +446,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11">
@@ -454,7 +454,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12">
@@ -462,7 +462,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13">
@@ -470,7 +470,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14">
@@ -478,7 +478,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15">
@@ -486,7 +486,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16">
@@ -494,7 +494,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17">
@@ -502,7 +502,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18">
@@ -510,7 +510,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19">
@@ -518,7 +518,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20">
@@ -526,7 +526,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21">
@@ -534,7 +534,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22">
@@ -542,7 +542,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23">
@@ -550,7 +550,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24">
@@ -558,7 +558,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25">
@@ -566,7 +566,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26">
@@ -711,7 +711,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3">
@@ -719,7 +719,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
@@ -727,7 +727,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5">
@@ -735,7 +735,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
@@ -743,7 +743,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7">
@@ -751,7 +751,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
@@ -759,7 +759,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9">
@@ -767,7 +767,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10">
@@ -775,7 +775,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11">
@@ -783,7 +783,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12">
@@ -791,7 +791,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13">
@@ -799,7 +799,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14">
@@ -807,7 +807,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15">
@@ -815,7 +815,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16">
@@ -823,7 +823,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17">
@@ -831,7 +831,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18">
@@ -839,7 +839,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19">
@@ -847,7 +847,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20">
@@ -855,7 +855,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21">
@@ -863,7 +863,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22">
@@ -871,7 +871,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23">
@@ -879,7 +879,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24">
@@ -887,7 +887,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25">
@@ -895,7 +895,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26">
@@ -903,7 +903,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27">
@@ -911,7 +911,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28">
@@ -919,7 +919,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29">
@@ -927,7 +927,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30">
@@ -1040,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3">
@@ -1048,7 +1048,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4">
@@ -1056,7 +1056,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5">
@@ -1064,7 +1064,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6">
@@ -1072,7 +1072,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7">
@@ -1080,7 +1080,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8">
@@ -1088,7 +1088,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9">
@@ -1096,7 +1096,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10">
@@ -1104,7 +1104,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11">
@@ -1112,7 +1112,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12">
@@ -1120,7 +1120,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13">
@@ -1136,7 +1136,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15">
@@ -1144,7 +1144,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16">
@@ -1152,7 +1152,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17">
@@ -1176,7 +1176,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20">
@@ -1184,7 +1184,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21">
@@ -1192,7 +1192,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22">
@@ -1200,7 +1200,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23">
@@ -1208,7 +1208,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24">
@@ -1216,7 +1216,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25">
@@ -1224,7 +1224,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26">
@@ -1232,7 +1232,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27">
@@ -1240,7 +1240,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28">
@@ -1248,7 +1248,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29">
@@ -1256,7 +1256,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30">
@@ -1264,7 +1264,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31">
@@ -1272,7 +1272,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32">
@@ -1280,7 +1280,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33">
@@ -1369,7 +1369,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
@@ -1377,7 +1377,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4">
@@ -1385,7 +1385,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
@@ -1393,7 +1393,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6">
@@ -1401,7 +1401,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7">
@@ -1409,7 +1409,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8">
@@ -1417,7 +1417,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9">
@@ -1425,7 +1425,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10">
@@ -1433,7 +1433,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11">
@@ -1441,7 +1441,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12">
@@ -1449,7 +1449,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13">
@@ -1457,7 +1457,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14">
@@ -1465,7 +1465,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15">
@@ -1473,7 +1473,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16">
@@ -1481,7 +1481,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17">
@@ -1489,7 +1489,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18">
@@ -1497,7 +1497,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19">
@@ -1505,7 +1505,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20">
@@ -1513,7 +1513,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21">
@@ -1521,7 +1521,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22">
@@ -1529,7 +1529,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23">
@@ -1537,7 +1537,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24">
@@ -1545,7 +1545,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25">
@@ -1593,7 +1593,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31">
@@ -1601,7 +1601,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32">
@@ -1609,7 +1609,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33">
@@ -1617,7 +1617,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34">
@@ -1625,7 +1625,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35">
@@ -1633,7 +1633,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36">
@@ -1641,7 +1641,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37">
@@ -1649,7 +1649,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38">
@@ -1698,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
@@ -1706,7 +1706,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
@@ -1714,7 +1714,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -1722,7 +1722,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
@@ -1730,7 +1730,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7">
@@ -1738,7 +1738,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8">
@@ -1746,7 +1746,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9">
@@ -1754,7 +1754,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10">
@@ -1762,7 +1762,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11">
@@ -1770,7 +1770,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12">
@@ -1778,7 +1778,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13">
@@ -1786,7 +1786,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14">
@@ -1794,7 +1794,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15">
@@ -1802,7 +1802,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16">
@@ -1810,7 +1810,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17">
@@ -1818,7 +1818,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18">
@@ -1826,7 +1826,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19">
@@ -1834,7 +1834,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20">
@@ -1842,7 +1842,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21">
@@ -1850,7 +1850,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22">
@@ -1858,7 +1858,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23">
@@ -1866,7 +1866,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24">
@@ -1874,7 +1874,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25">
@@ -1882,7 +1882,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26">
@@ -1890,7 +1890,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27">
@@ -1898,7 +1898,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28">
@@ -1906,7 +1906,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29">
@@ -1914,7 +1914,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30">
@@ -1922,7 +1922,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31">
@@ -1930,7 +1930,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32">
@@ -1938,7 +1938,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33">
@@ -1946,7 +1946,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34">
@@ -1954,7 +1954,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35">
@@ -1986,7 +1986,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39">
@@ -1994,7 +1994,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2027,7 +2027,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
@@ -2035,7 +2035,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4">
@@ -2043,7 +2043,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
@@ -2051,7 +2051,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
@@ -2059,7 +2059,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7">
@@ -2067,7 +2067,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
@@ -2075,7 +2075,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
@@ -2083,7 +2083,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10">
@@ -2091,7 +2091,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11">
@@ -2099,7 +2099,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12">
@@ -2107,7 +2107,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
@@ -2115,7 +2115,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14">
@@ -2123,7 +2123,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
@@ -2131,7 +2131,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16">
@@ -2139,7 +2139,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
@@ -2147,7 +2147,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -2155,7 +2155,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19">
@@ -2163,7 +2163,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20">
@@ -2171,7 +2171,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21">
@@ -2179,7 +2179,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22">
@@ -2195,7 +2195,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24">
@@ -2203,7 +2203,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25">
@@ -2211,7 +2211,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26">
@@ -2219,7 +2219,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27">
@@ -2227,7 +2227,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28">
@@ -2235,7 +2235,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29">
@@ -2243,7 +2243,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30">
@@ -2251,7 +2251,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31">
@@ -2259,7 +2259,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32">
@@ -2267,7 +2267,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33">
@@ -2275,7 +2275,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34">
@@ -2283,7 +2283,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35">
@@ -2291,7 +2291,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36">
@@ -2299,7 +2299,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37">
@@ -2307,7 +2307,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38">
@@ -2315,7 +2315,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39">
@@ -2323,7 +2323,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2356,7 +2356,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
@@ -2364,7 +2364,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
@@ -2372,7 +2372,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -2380,7 +2380,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
@@ -2388,7 +2388,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
@@ -2396,7 +2396,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8">
@@ -2404,7 +2404,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9">
@@ -2412,7 +2412,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10">
@@ -2420,7 +2420,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11">
@@ -2428,7 +2428,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12">
@@ -2436,7 +2436,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13">
@@ -2444,7 +2444,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14">
@@ -2452,7 +2452,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15">
@@ -2460,7 +2460,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16">
@@ -2468,7 +2468,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17">
@@ -2476,7 +2476,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18">
@@ -2516,7 +2516,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23">
@@ -2532,7 +2532,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25">
@@ -2540,7 +2540,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26">
@@ -2548,7 +2548,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27">
@@ -2556,7 +2556,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28">
@@ -2564,7 +2564,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29">
@@ -2572,7 +2572,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30">
@@ -2580,7 +2580,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31">
@@ -2588,7 +2588,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32">
@@ -2596,7 +2596,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33">
@@ -2604,7 +2604,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34">
@@ -2612,7 +2612,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35">
@@ -2620,7 +2620,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36">
@@ -2644,7 +2644,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39">
@@ -2652,7 +2652,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2685,7 +2685,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
@@ -2693,7 +2693,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -2701,7 +2701,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5">
@@ -2709,7 +2709,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6">
@@ -2717,7 +2717,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">
@@ -2725,7 +2725,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8">
@@ -2733,7 +2733,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9">
@@ -2741,7 +2741,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10">
@@ -2749,7 +2749,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11">
@@ -2757,7 +2757,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
@@ -2765,7 +2765,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13">
@@ -2773,7 +2773,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14">
@@ -2781,7 +2781,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15">
@@ -2813,7 +2813,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19">
@@ -2821,7 +2821,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20">
@@ -2829,7 +2829,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21">
@@ -2837,7 +2837,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22">
@@ -2845,7 +2845,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23">
@@ -2853,7 +2853,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24">
@@ -2861,7 +2861,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25">
@@ -2869,7 +2869,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26">
@@ -2877,7 +2877,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27">
@@ -2885,7 +2885,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28">
@@ -2893,7 +2893,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29">
@@ -2901,7 +2901,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30">
@@ -2909,7 +2909,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31">
@@ -2917,7 +2917,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32">
@@ -2925,7 +2925,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33">
@@ -2933,7 +2933,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34">
@@ -2941,7 +2941,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35">
@@ -2949,7 +2949,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36">
@@ -2957,7 +2957,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37">
@@ -2965,7 +2965,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38">
@@ -2973,7 +2973,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39">
@@ -2981,7 +2981,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3014,7 +3014,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3">
@@ -3022,7 +3022,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4">
@@ -3030,7 +3030,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
@@ -3038,7 +3038,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6">
@@ -3046,7 +3046,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7">
@@ -3054,7 +3054,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8">
@@ -3062,7 +3062,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9">
@@ -3070,7 +3070,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10">
@@ -3078,7 +3078,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11">
@@ -3086,7 +3086,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
@@ -3094,7 +3094,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13">
@@ -3102,7 +3102,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14">
@@ -3118,7 +3118,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16">
@@ -3126,7 +3126,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17">
@@ -3134,7 +3134,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18">
@@ -3142,7 +3142,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19">
@@ -3150,7 +3150,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20">
@@ -3158,7 +3158,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21">
@@ -3166,7 +3166,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22">
@@ -3174,7 +3174,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23">
@@ -3182,7 +3182,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24">
@@ -3190,7 +3190,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25">
@@ -3198,7 +3198,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26">
@@ -3206,7 +3206,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27">
@@ -3214,7 +3214,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28">
@@ -3222,7 +3222,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29">
@@ -3230,7 +3230,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30">
@@ -3238,7 +3238,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31">
@@ -3246,7 +3246,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>113</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32">
@@ -3254,7 +3254,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>113</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33">
@@ -3262,7 +3262,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>113</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34">
@@ -3270,7 +3270,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>113</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35">
@@ -3278,7 +3278,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>113</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36">
@@ -3286,7 +3286,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>113</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37">
@@ -3294,7 +3294,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>113</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38">
@@ -3302,7 +3302,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39">
@@ -3310,7 +3310,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>